<commit_message>
add "total" line at the end
</commit_message>
<xml_diff>
--- a/reports/clslab-liquid-bom.xlsx
+++ b/reports/clslab-liquid-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\sparks-baird\self-driving-lab-demo\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\self-driving-lab-demo\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6006C62-699E-45E8-9F99-A3FB7676E10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043D736E-C25A-419E-AD47-E9BF1D7B3F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E91E5351-9248-443C-8FD2-9FE695AF132B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E91E5351-9248-443C-8FD2-9FE695AF132B}"/>
   </bookViews>
   <sheets>
     <sheet name="bill-of-materials" sheetId="1" r:id="rId1"/>
@@ -777,8 +777,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -836,14 +836,15 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1160,25 +1161,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1639D2-2D5B-4478-B0D8-EB00226620F8}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="89.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>114</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -1345,7 +1346,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>162</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -1609,7 +1610,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>152</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -1825,10 +1826,16 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E30" s="4">
+        <f>SUM(E2:E27)</f>
+        <v>290.8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1867,16 +1874,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A83F356-DA6A-40F7-B586-1DCB5C35EB75}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>137</v>
       </c>
@@ -1896,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1938,7 +1945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1959,7 +1966,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1980,7 +1987,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2001,7 +2008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2022,7 +2029,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2043,7 +2050,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2064,7 +2071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2085,7 +2092,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2106,7 +2113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2127,7 +2134,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2155,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2169,7 +2176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -2211,7 +2218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -2232,7 +2239,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -2253,7 +2260,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2295,7 +2302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2316,7 +2323,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2337,7 +2344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>112</v>
       </c>
@@ -2358,7 +2365,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -2379,7 +2386,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2400,7 +2407,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -2463,7 +2470,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2484,7 +2491,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -2505,7 +2512,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -2526,7 +2533,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -2547,7 +2554,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
fix out of stock links
</commit_message>
<xml_diff>
--- a/reports/clslab-liquid-bom.xlsx
+++ b/reports/clslab-liquid-bom.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\self-driving-lab-demo\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE89D58-79FF-45C7-9B24-180BC9964687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018039DC-5F48-4A36-BF8A-0AEF87F2B580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E91E5351-9248-443C-8FD2-9FE695AF132B}"/>
   </bookViews>
   <sheets>
     <sheet name="bill-of-materials" sheetId="1" r:id="rId1"/>
-    <sheet name="extras-alternatives" sheetId="3" r:id="rId2"/>
+    <sheet name="extras" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'bill-of-materials'!$A$1:$H$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">extras!$A$1:$H$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -126,7 +127,7 @@
     <author>Sterling Baird</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{40D42F2B-A357-45AF-B228-B53CA4F4BD42}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{058B418B-4FB8-4D22-8402-7AFAFE0F9C4A}">
       <text>
         <r>
           <rPr>
@@ -150,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{AC4CB2CE-578A-452E-955B-55B4D66B0275}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{1B914C78-3DB8-4ED7-BE0B-629F28E3C4FF}">
       <text>
         <r>
           <rPr>
@@ -174,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{EE830F69-BA81-4FA0-80EB-F66E50F8DBB3}">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{C7A5CCA6-7F16-416A-BF30-9709689F0B3D}">
       <text>
         <r>
           <rPr>
@@ -198,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{8BF7E175-44C1-411B-BAF5-1B809E7A0E08}">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{F4ABD14C-0B03-4E29-B8C5-EFD183B9E3C4}">
       <text>
         <r>
           <rPr>
@@ -222,7 +223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{B1583AB1-11CF-4FBB-BDAF-297BA349DDB9}">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{C61F9E9E-49B7-4EDA-AB53-FBDF61532DE7}">
       <text>
         <r>
           <rPr>
@@ -246,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{0039889F-E207-4F68-AE59-28278C393A81}">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{F43A8041-822D-4939-85D5-8D73EBFCAE54}">
       <text>
         <r>
           <rPr>
@@ -275,29 +276,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="192">
   <si>
     <t>Sculpting wire</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/gp/product/B0B11VW3NG</t>
   </si>
   <si>
@@ -316,9 +299,6 @@
     <t>Raspberry Pi Pico W</t>
   </si>
   <si>
-    <t>Pishop</t>
-  </si>
-  <si>
     <t>Raspberry Pi Pico W and loose headers</t>
   </si>
   <si>
@@ -328,9 +308,6 @@
     <t>https://www.digikey.com/en/products/detail/cytron-technologies-sdn-bhd/MAKER-PI-PICO-NB/14557835</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>DC Motor Driver Module for Raspberry Pi Pico</t>
   </si>
   <si>
@@ -340,9 +317,6 @@
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4698/13162109</t>
   </si>
   <si>
-    <t>Waveshare</t>
-  </si>
-  <si>
     <t>https://www.waveshare.com/pico-motor-driver.htm</t>
   </si>
   <si>
@@ -397,9 +371,6 @@
     <t>Both ends open quartz cuvette</t>
   </si>
   <si>
-    <t>ecuvette</t>
-  </si>
-  <si>
     <t>Cuvette lid</t>
   </si>
   <si>
@@ -430,9 +401,6 @@
     <t>https://www.freshwatersystems.com/products/dmfit-two-way-divider-1-4-x-1-4-x-1-4-push-in?variant=13249525121067</t>
   </si>
   <si>
-    <t>amazon</t>
-  </si>
-  <si>
     <t>Splitter (pack of 10)</t>
   </si>
   <si>
@@ -788,6 +756,102 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>wire_strippers</t>
+  </si>
+  <si>
+    <t>slotted_screwdriver</t>
+  </si>
+  <si>
+    <t>solder_iron</t>
+  </si>
+  <si>
+    <t>grove_to_female</t>
+  </si>
+  <si>
+    <t>sculpting_wire</t>
+  </si>
+  <si>
+    <t>silicone_tubing_10ft</t>
+  </si>
+  <si>
+    <t>epoxy</t>
+  </si>
+  <si>
+    <t>dc_motor_driver</t>
+  </si>
+  <si>
+    <t>jumper_cable_20pin</t>
+  </si>
+  <si>
+    <t>grove_connectors</t>
+  </si>
+  <si>
+    <t>glass_cuvette_sealing_lid</t>
+  </si>
+  <si>
+    <t>water_splitter_4mm</t>
+  </si>
+  <si>
+    <t>ptfe_tubing_2mm_4mm</t>
+  </si>
+  <si>
+    <t>straight_union_fitting_4mm</t>
+  </si>
+  <si>
+    <t>jack_to_open_wire_2.1mm</t>
+  </si>
+  <si>
+    <t>cuvette_lid</t>
+  </si>
+  <si>
+    <t>quartz_cuvette_open_ends</t>
+  </si>
+  <si>
+    <t>grove_relay_connector</t>
+  </si>
+  <si>
+    <t>hose_clamp</t>
+  </si>
+  <si>
+    <t>push_to_connect_reducer_6mm_4mm</t>
+  </si>
+  <si>
+    <t>water_splitter_0.25in</t>
+  </si>
+  <si>
+    <t>dc_power_adapter_female</t>
+  </si>
+  <si>
+    <t>stacking_header</t>
+  </si>
+  <si>
+    <t>water_splitter_freshwater</t>
+  </si>
+  <si>
+    <t>water_splitter_amazon</t>
+  </si>
+  <si>
+    <t>pico_w_loose_headers</t>
+  </si>
+  <si>
+    <t>quartz_cuvette_2pk</t>
+  </si>
+  <si>
+    <t>power_splitter_2_way</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Sandpaper-Furniture-Finishing-Automotive-Polishing/dp/B09821SB56/</t>
+  </si>
+  <si>
+    <t>Sandpaper 120 Grit, Wet Dry Sanding Sheets 9 x 11 Inch, 12 sheets</t>
+  </si>
+  <si>
+    <t>AHOUGER 4Pcs 3.5L Plant Life Drip Watering Bag with Adjustable Flow</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AHOUGER-Watering-Planter-Automatic-Irrigation/dp/B09G6KJ3PV/</t>
   </si>
 </sst>
 </file>
@@ -872,7 +936,49 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -920,11 +1026,22 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -951,9 +1068,29 @@
     <tableColumn id="3" xr3:uid="{341E8280-F9C6-4368-8CF2-FA06D12092D3}" name="Component"/>
     <tableColumn id="4" xr3:uid="{1C2B67A7-E979-4570-A5AE-3F9F8ED11D6D}" name="Number"/>
     <tableColumn id="5" xr3:uid="{E9A68000-FD58-41C1-B10E-E71D1E23C920}" name="Cost per unit - currency"/>
-    <tableColumn id="6" xr3:uid="{CD3FB727-7F7F-483D-836A-924928CC7DB8}" name="Total cost - currency" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{CD3FB727-7F7F-483D-836A-924928CC7DB8}" name="Total cost - currency" dataDxfId="11" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{E2CEB878-6AE7-4401-A20F-64F5693AA456}" name="Source of materials" dataCellStyle="Hyperlink"/>
     <tableColumn id="8" xr3:uid="{D9E42E9B-7D5D-46E6-A150-6BB57D8FE728}" name="Material type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94B8D685-3B2C-4D72-8753-9B23957BDCDA}" name="Table13" displayName="Table13" ref="A1:H40" totalsRowShown="0">
+  <autoFilter ref="A1:H40" xr:uid="{3B1639D2-2D5B-4478-B0D8-EB00226620F8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H40">
+    <sortCondition ref="A1:A40"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{EE6F9C85-1C9D-45E7-B804-C9786D5E98D3}" name="CLSLab:Light"/>
+    <tableColumn id="2" xr3:uid="{54508CF3-EBAC-49ED-9DD3-BA93EF46997B}" name="Designator"/>
+    <tableColumn id="3" xr3:uid="{C47D367F-0AEE-4073-AE7F-625D4F05CC16}" name="Component"/>
+    <tableColumn id="4" xr3:uid="{5525CA8A-BDAD-41DD-A630-22C3F7E65B19}" name="Number"/>
+    <tableColumn id="5" xr3:uid="{068E2C7E-E523-437B-8FBE-38E0230373A3}" name="Cost per unit - currency"/>
+    <tableColumn id="6" xr3:uid="{D3102271-CB8F-46AC-B399-82D7A41BC5A9}" name="Total cost - currency" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{969A2974-1F6C-4DA6-B6AF-C4F4F34A797F}" name="Source of materials" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{F48A9C56-2406-45EB-91A8-0623E89EB40B}" name="Material type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1260,7 +1397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,66 +1414,63 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>190</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>20.99</v>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>22.99</v>
       </c>
       <c r="F2" s="2">
         <f>D2*E2</f>
-        <v>20.99</v>
+        <v>45.98</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1349,21 +1483,21 @@
         <v>18.91</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1376,21 +1510,21 @@
         <v>16.09</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1403,21 +1537,21 @@
         <v>12.99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1430,21 +1564,21 @@
         <v>59.900000000000006</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1457,21 +1591,21 @@
         <v>10.99</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1484,21 +1618,21 @@
         <v>9.99</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="H8" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1511,48 +1645,45 @@
         <v>9.99</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>6.99</v>
+        <v>10.97</v>
       </c>
       <c r="F10" s="2">
         <f>D10*E10</f>
-        <v>6.99</v>
+        <v>10.97</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1565,21 +1696,21 @@
         <v>6.99</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1592,21 +1723,21 @@
         <v>20.700000000000003</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1619,48 +1750,45 @@
         <v>9.9600000000000009</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H13" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>4.95</v>
+        <v>2.95</v>
       </c>
       <c r="F14" s="2">
         <f>D14*E14</f>
-        <v>4.95</v>
+        <v>2.95</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" t="s">
-        <v>146</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1673,21 +1801,21 @@
         <v>4.79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1700,21 +1828,21 @@
         <v>2.86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1727,21 +1855,21 @@
         <v>2.1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1754,21 +1882,21 @@
         <v>6</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1781,21 +1909,21 @@
         <v>24.12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1808,21 +1936,21 @@
         <v>15.95</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1835,18 +1963,18 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1859,21 +1987,21 @@
         <v>8.4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1886,21 +2014,21 @@
         <v>3.95</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H23" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1913,21 +2041,21 @@
         <v>2.58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1940,21 +2068,21 @@
         <v>1.95</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -1967,10 +2095,10 @@
         <v>1.8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H26" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1981,12 +2109,42 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F29" s="4">
         <f>SUM(F2:F26)</f>
-        <v>293.74</v>
+        <v>320.70999999999998</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:H45">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A15:H45 A3:H9 A11:H13 E11:F26">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$A3="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>$A14="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:E10 G10:H10">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>$A10="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>$A10="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:H2 B2:E2">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>$A2="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$A2="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$A2="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1994,823 +2152,1000 @@
     <hyperlink ref="G25" r:id="rId1" xr:uid="{C5F6E3A1-832E-4FD5-8BD6-FC546B0FDAB6}"/>
     <hyperlink ref="G22" r:id="rId2" xr:uid="{B2BE2E68-1D25-4529-8255-9B059365EF39}"/>
     <hyperlink ref="G17" r:id="rId3" xr:uid="{5854D339-2716-49B9-BE3E-FADE32F53000}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{9DF5D0B0-A815-4C20-8059-E1B426A08B82}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{D5056138-7C85-4971-B051-7CDFD5AB73F6}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{68FDB5F7-38DB-4A82-9B0F-8920FBD9E2E2}"/>
-    <hyperlink ref="G15" r:id="rId7" xr:uid="{0152A3F6-FE58-41D7-AB64-C8E374049A9A}"/>
-    <hyperlink ref="G20" r:id="rId8" xr:uid="{2976C01C-06EF-45D8-BDD8-2D85223A5AF6}"/>
-    <hyperlink ref="G24" r:id="rId9" xr:uid="{5E3C4CA6-3F8C-4365-A6C1-0A55444B5309}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{E84B8222-0F2B-442C-B630-DB5345EB5421}"/>
-    <hyperlink ref="G8" r:id="rId11" xr:uid="{CE847A67-9E0A-4400-8F59-D5077969B9D4}"/>
-    <hyperlink ref="G5" r:id="rId12" xr:uid="{144AF5F5-759F-4E3A-88EE-13D15BFE0C3D}"/>
-    <hyperlink ref="G10" r:id="rId13" xr:uid="{3045F596-E1FC-4E95-8F05-3577A230B8B5}"/>
-    <hyperlink ref="G14" r:id="rId14" xr:uid="{FE6399ED-A3BE-4760-BF33-77FE544C9E60}"/>
-    <hyperlink ref="G4" r:id="rId15" xr:uid="{EF01DC0F-F8AB-4EDD-B512-EA3EC5D82508}"/>
-    <hyperlink ref="G9" r:id="rId16" xr:uid="{51A13458-B9B3-472F-A80F-93724CE2E51F}"/>
-    <hyperlink ref="G18" r:id="rId17" xr:uid="{27CCFCFD-9EA7-46FB-AB4E-1F287FBE0A22}"/>
-    <hyperlink ref="G26" r:id="rId18" xr:uid="{9E35136C-306F-4B70-8108-BB61C7C23A40}"/>
-    <hyperlink ref="G23" r:id="rId19" xr:uid="{F4046E26-D68C-4E6C-840B-4F4805F69E12}"/>
-    <hyperlink ref="G19" r:id="rId20" xr:uid="{0C41FF5B-1F3C-46B2-883B-1F9FA1730239}"/>
-    <hyperlink ref="G16" r:id="rId21" xr:uid="{2ED3E1C8-999F-43C5-92EF-A1A86B17F428}"/>
-    <hyperlink ref="G7" r:id="rId22" xr:uid="{114442ED-270E-4449-9415-FCDF80A1E50C}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{D5056138-7C85-4971-B051-7CDFD5AB73F6}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{68FDB5F7-38DB-4A82-9B0F-8920FBD9E2E2}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{0152A3F6-FE58-41D7-AB64-C8E374049A9A}"/>
+    <hyperlink ref="G20" r:id="rId7" xr:uid="{2976C01C-06EF-45D8-BDD8-2D85223A5AF6}"/>
+    <hyperlink ref="G24" r:id="rId8" xr:uid="{5E3C4CA6-3F8C-4365-A6C1-0A55444B5309}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{E84B8222-0F2B-442C-B630-DB5345EB5421}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{CE847A67-9E0A-4400-8F59-D5077969B9D4}"/>
+    <hyperlink ref="G5" r:id="rId11" xr:uid="{144AF5F5-759F-4E3A-88EE-13D15BFE0C3D}"/>
+    <hyperlink ref="G4" r:id="rId12" xr:uid="{EF01DC0F-F8AB-4EDD-B512-EA3EC5D82508}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{51A13458-B9B3-472F-A80F-93724CE2E51F}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{27CCFCFD-9EA7-46FB-AB4E-1F287FBE0A22}"/>
+    <hyperlink ref="G26" r:id="rId15" xr:uid="{9E35136C-306F-4B70-8108-BB61C7C23A40}"/>
+    <hyperlink ref="G23" r:id="rId16" xr:uid="{F4046E26-D68C-4E6C-840B-4F4805F69E12}"/>
+    <hyperlink ref="G19" r:id="rId17" xr:uid="{0C41FF5B-1F3C-46B2-883B-1F9FA1730239}"/>
+    <hyperlink ref="G16" r:id="rId18" xr:uid="{2ED3E1C8-999F-43C5-92EF-A1A86B17F428}"/>
+    <hyperlink ref="G7" r:id="rId19" xr:uid="{114442ED-270E-4449-9415-FCDF80A1E50C}"/>
+    <hyperlink ref="G14" r:id="rId20" xr:uid="{37561F33-C53A-46A0-946C-6963962397AD}"/>
+    <hyperlink ref="G2" r:id="rId21" xr:uid="{D97E0D36-23C0-46A8-88E1-A7CBC26C3AC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
+  <legacyDrawing r:id="rId23"/>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A83F356-DA6A-40F7-B586-1DCB5C35EB75}">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DF9F76-D3FC-49B6-AE66-137E06C1E68F}">
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>39.99</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*E2</f>
+        <v>39.99</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3*E3</f>
+        <v>7.95</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="F4" s="2">
+        <f>D4*E4</f>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>23.1</v>
+      </c>
+      <c r="F5" s="2">
+        <f>D5*E5</f>
+        <v>23.1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="2">
+        <f>D6*E6</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7*E7</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F8" s="2">
+        <f>D8*E8</f>
+        <v>7.99</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="F9" s="2">
+        <f>D9*E9</f>
+        <v>6.99</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F10" s="2">
+        <f>D10*E10</f>
+        <v>7.99</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="F11" s="2">
+        <f>D11*E11</f>
+        <v>3.2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2">
+        <f>D12*E12</f>
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <f>D13*E13</f>
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3.31</v>
+      </c>
+      <c r="F14" s="2">
+        <f>D14*E14</f>
+        <v>3.31</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>7.29</v>
+      </c>
+      <c r="F15" s="2">
+        <f>D15*E15</f>
+        <v>7.29</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="F16" s="2">
+        <f>D16*E16</f>
+        <v>8.99</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F17" s="2">
+        <f>D17*E17</f>
+        <v>7.99</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>29.99</v>
+      </c>
+      <c r="F18" s="2">
+        <f>D18*E18</f>
+        <v>29.99</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="F19" s="2">
+        <f>D19*E19</f>
+        <v>2.1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="F20" s="2">
+        <f>D20*E20</f>
+        <v>3.9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F21" s="2">
+        <f>D21*E21</f>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7.47</v>
+      </c>
+      <c r="F22" s="2">
+        <f>D22*E22</f>
+        <v>7.47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F23" s="2">
+        <f>D23*E23</f>
+        <v>7.99</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="F24" s="2">
+        <f>D24*E24</f>
+        <v>7.99</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="F25" s="2">
+        <f>D25*E25</f>
+        <v>10.99</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F26" s="2">
+        <f>D26*E26</f>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>20.99</v>
+      </c>
+      <c r="F27" s="2">
+        <f>D27*E27</f>
+        <v>20.99</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="F28" s="2">
+        <f>D28*E28</f>
+        <v>4.3</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>7.77</v>
+      </c>
+      <c r="F29" s="2">
+        <f>D29*E29</f>
+        <v>7.77</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="F30" s="2">
+        <f>D30*E30</f>
+        <v>4.95</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="F31" s="2">
+        <f>D31*E31</f>
+        <v>3.99</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="F32" s="2">
+        <f>D32*E32</f>
+        <v>8.99</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>6</v>
+      </c>
+      <c r="F33" s="2">
+        <f>D33*E33</f>
+        <v>6</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F34" s="2">
+        <f>D34*E34</f>
+        <v>0.86</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="F35" s="2">
+        <f>D35*E35</f>
+        <v>4.95</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="F37" s="2">
+        <f>D37*E37</f>
+        <v>6.99</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" t="s">
         <v>137</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>39.99</v>
-      </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:E3" si="0">C2*D2</f>
-        <v>39.99</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>7.95</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" si="0"/>
-        <v>7.95</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4:E9" si="1">C4*D4</f>
-        <v>3.9000000000000004</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>23.1</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="1"/>
-        <v>23.1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7.99</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="1"/>
-        <v>7.99</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>6.99</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="1"/>
-        <v>6.99</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7.99</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" ref="E10:E16" si="2">C10*D10</f>
-        <v>7.99</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="2"/>
-        <v>3.2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>27</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3.31</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="2"/>
-        <v>3.31</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>7.29</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="2"/>
-        <v>7.29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>8.99</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="2"/>
-        <v>8.99</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>7.99</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" ref="E17:E32" si="3">C17*D17</f>
-        <v>7.99</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3">
-        <v>29.99</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="3"/>
-        <v>29.99</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="3"/>
-        <v>2.1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1.95</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="3"/>
-        <v>3.9</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>19.989999999999998</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="3"/>
-        <v>19.989999999999998</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>7.47</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="3"/>
-        <v>7.47</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>7.99</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="3"/>
-        <v>7.99</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>7.99</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" si="3"/>
-        <v>7.99</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>8.99</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="3"/>
-        <v>8.99</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="3"/>
+      <c r="F39" s="2">
+        <f>D39*E39</f>
         <v>0</v>
       </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2">
-        <v>10.99</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="3"/>
-        <v>10.99</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3">
-        <v>19.989999999999998</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="3"/>
-        <v>19.989999999999998</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3">
-        <v>2.95</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="3"/>
-        <v>2.95</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="E29" s="2">
-        <f t="shared" si="3"/>
-        <v>4.3</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <v>7.77</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" si="3"/>
-        <v>7.77</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="3">
-        <v>4.95</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="3"/>
-        <v>4.95</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3.99</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="3"/>
-        <v>3.99</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>8.99</v>
-      </c>
-      <c r="E33" s="2">
-        <f>C33*D33</f>
-        <v>8.99</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2">
-        <v>6</v>
-      </c>
-      <c r="E34" s="2">
-        <f>C34*D34</f>
-        <v>6</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.43</v>
-      </c>
-      <c r="E35" s="2">
-        <f>C35*D35</f>
-        <v>0.86</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" t="s">
-        <v>146</v>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F40" s="4">
+        <f>SUM(F2:F37)</f>
+        <v>344.89000000000004</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A40:H56 G39:H39 A39:E39 A28:A34 A2:A26 A35:D35 G35:H35 E2:F26 E28:F35 A37:H37 A27:H27">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>$A2="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>$A39="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{07AFA779-ED68-4644-A33E-A1F31DDF7CC1}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{A5DA8DD3-AB98-42E8-B3AE-4E6819E1B4EC}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{07FD9283-54AE-4833-92BB-F78B78140EFB}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{916C66BC-B961-46E5-B199-EE47029CFC21}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{638763E9-0861-4A1D-B20B-B810BFBAEFC4}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{ECDB46F1-EBB3-411C-B2AD-C38C9CB12B08}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{978E1A70-BD8B-4D1D-BD98-CC1E2572F3C0}"/>
-    <hyperlink ref="F11" r:id="rId8" xr:uid="{C5189A0F-6A1E-4EB7-B0EE-C9F9C31F6FB6}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{20BC59A6-3E21-499D-A3BE-7F4688DB7669}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{F1BA0C61-5376-465D-AB06-5E01E2179041}"/>
-    <hyperlink ref="F14" r:id="rId11" xr:uid="{44ABE6CD-4E6D-475A-842D-942166C3FA57}"/>
-    <hyperlink ref="F15" r:id="rId12" xr:uid="{4DE7DCA4-77B8-482E-BFB8-69ABFDAB9416}"/>
-    <hyperlink ref="F16" r:id="rId13" xr:uid="{E8DFC8C8-BFC9-4762-A5A9-0C0D8B61A3AD}"/>
-    <hyperlink ref="F17" r:id="rId14" xr:uid="{3CC123F2-E5F2-4C35-9A60-9135FDA068E1}"/>
-    <hyperlink ref="F18" r:id="rId15" xr:uid="{55FD34F5-30B7-4FD2-8D08-04AACC942CC8}"/>
-    <hyperlink ref="F19" r:id="rId16" xr:uid="{A301E5AB-D96F-4BE1-B641-8D31C07525C1}"/>
-    <hyperlink ref="F20" r:id="rId17" xr:uid="{05EAFDB5-3875-46D6-B581-FDA74FFB5E3A}"/>
-    <hyperlink ref="F21" r:id="rId18" xr:uid="{DACE2763-167E-40B2-93F9-D48B12FF6263}"/>
-    <hyperlink ref="F22" r:id="rId19" xr:uid="{9283A10A-E872-4DFA-B921-43BB3BB2A9D1}"/>
-    <hyperlink ref="F23" r:id="rId20" xr:uid="{4EBD25A6-BC90-4F48-8400-2D5D15DB67BB}"/>
-    <hyperlink ref="F24" r:id="rId21" xr:uid="{C54DA0C4-0210-4120-8B27-966398DA9148}"/>
-    <hyperlink ref="F25" r:id="rId22" xr:uid="{75173C7D-D480-4C2D-BE5A-040CEC28705B}"/>
-    <hyperlink ref="F27" r:id="rId23" xr:uid="{D3B96166-191E-4925-B576-8152A865AF7F}"/>
-    <hyperlink ref="F28" r:id="rId24" xr:uid="{857530DA-12FF-4E18-8DF7-C2A81B84228F}"/>
-    <hyperlink ref="F26" r:id="rId25" xr:uid="{9A0672E1-2100-4676-B1ED-912FF121366A}"/>
-    <hyperlink ref="F33" r:id="rId26" xr:uid="{BFEA466E-9D75-4187-B0D2-9339C28C2E2C}"/>
-    <hyperlink ref="F34" r:id="rId27" xr:uid="{A1D5FB76-9E48-42F1-9287-96810421B11C}"/>
-    <hyperlink ref="F35" r:id="rId28" xr:uid="{ABA147CF-4F75-447A-A717-A1AEC4AB0096}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{FB8340EE-5DB1-45BF-B700-EEF911451C61}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{F569E00B-93FE-4224-A3E1-4EFE351FF9FE}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{EF2D723A-780B-459A-AE0B-D2CAE73741F0}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{0820405B-FF80-417A-AC5F-B951EBB3B7FA}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{9102718A-BD3B-44DA-95BE-7D1863FE221F}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{555EE6EF-DA77-4FF3-9F73-303A93DB2844}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{FC8E5874-8037-4EA5-A2C1-C27CBC8F20D8}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{96DD20F5-0478-46BB-8253-1A45B62A05E3}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{9F296F62-AFBE-4E3F-AE68-1AB4AB63E7CC}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{E25B0DFD-6119-4275-8667-41A654BF0A54}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{331B9BA5-C6BF-4AA0-9BE4-3214FBC05DFC}"/>
+    <hyperlink ref="G15" r:id="rId12" xr:uid="{68E8946A-E8E4-40FD-BC8B-429A81DE44C2}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{1878BC74-B7D4-48BA-BD41-A06A16D07957}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{DD8ECB28-A1FF-4598-9195-897CE68C0C9E}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{6998130E-E9E8-4E3E-8856-1CB8F7767B66}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{2A80EA26-BC05-4AE6-9CF5-B9CC3655E544}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{7D1A334A-5077-4D79-BA6C-0C96EF97F3F7}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{4FEA271B-44B8-4C3C-98DE-C4DD7DA68B62}"/>
+    <hyperlink ref="G22" r:id="rId19" xr:uid="{A6A27B30-8FD0-4ADA-B7FF-17C7E9B0241D}"/>
+    <hyperlink ref="G23" r:id="rId20" xr:uid="{066ACB74-13D8-46E6-AF35-006C466E63D2}"/>
+    <hyperlink ref="G24" r:id="rId21" xr:uid="{CDD7A05D-9D2B-480F-8971-354679B09556}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{DCB127EF-C9F4-42B9-979C-9CE31ACF274A}"/>
+    <hyperlink ref="G25" r:id="rId23" xr:uid="{A2B19890-F9CA-465C-B3E5-115D563E8112}"/>
+    <hyperlink ref="G32" r:id="rId24" xr:uid="{8EC6A34D-9B25-4B4A-8AC9-FEA32427D413}"/>
+    <hyperlink ref="G33" r:id="rId25" xr:uid="{A21CD645-5D93-4928-88D3-A1C760354A85}"/>
+    <hyperlink ref="G34" r:id="rId26" xr:uid="{32FAA24A-5420-4770-B649-1D25340FFE63}"/>
+    <hyperlink ref="G35" r:id="rId27" xr:uid="{FE6399ED-A3BE-4760-BF33-77FE544C9E60}"/>
+    <hyperlink ref="G37" r:id="rId28" xr:uid="{3045F596-E1FC-4E95-8F05-3577A230B8B5}"/>
+    <hyperlink ref="G27" r:id="rId29" xr:uid="{636D84C2-B4D9-4BA2-A219-BA4AF500FB59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
+  <legacyDrawing r:id="rId31"/>
+  <tableParts count="1">
+    <tablePart r:id="rId32"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>